<commit_message>
Deploying to gh-pages from  @ 0b8cb15958c6be7b9942b673aac4eb8d254d29ab 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_1-1-1.xlsx
+++ b/assets/excel/2022_1-1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1A68EE-6BE1-4BEB-ACD9-D21E895917A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9761549-CB06-4B29-B448-25A4F20D9B6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{61A8B6FB-8F47-4AE9-B753-E1770030DEA3}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Kreisfreie Stadt
 Landkreis
@@ -232,6 +232,18 @@
   <si>
     <t>Tabelle 1.1.1: Bevölkerung 2005 bis 2021</t>
   </si>
+  <si>
+    <t>Niedersächsisches Ministerium für Soziales, Gesundheit und Gleichstellung (Hrsg.),</t>
+  </si>
+  <si>
+    <t>© Landesamt für Statistik Niedersachsen, Hannover 2022,                                                                          </t>
+  </si>
+  <si>
+    <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangabe gestattet.</t>
+  </si>
+  <si>
+    <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
 </sst>
 </file>
 
@@ -241,7 +253,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="###\ ###\ ###"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,22 +290,40 @@
       <sz val="11"/>
       <name val="NDSFrutiger 55 Roman"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 55 Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 55 Roman"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="6"/>
+      <color theme="10"/>
+      <name val="NDSFrutiger 45 Light"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -384,12 +414,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -405,6 +445,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,12 +465,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{7F8ECBDE-67B2-4EBA-805E-8AAB15368B9E}"/>
   </cellStyles>
@@ -846,10 +905,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B011E5D6-05D1-40C2-9D08-6C21DEF65FF5}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:V67"/>
+  <dimension ref="B1:V71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,36 +934,36 @@
       </c>
     </row>
     <row r="7" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="10" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="6">
         <v>2005</v>
       </c>
@@ -967,31 +1026,31 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="10" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
@@ -1077,56 +1136,56 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="8">
         <v>245273</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="8">
         <v>245467</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="8">
         <v>245810</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="8">
         <v>246012</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="8">
         <v>247400</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="8">
         <v>248867</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="8">
         <v>243829</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="8">
         <v>245798</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="8">
         <v>247227</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="8">
         <v>248502</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="8">
         <v>251364</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="8">
         <v>248667</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="8">
         <v>248023</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="8">
         <v>248292</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="Q11" s="8">
         <v>249406</v>
       </c>
-      <c r="R11" s="14">
+      <c r="R11" s="8">
         <v>248561</v>
       </c>
       <c r="S11" s="15">
@@ -1142,56 +1201,56 @@
         <v>0.10540672108657433</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+    <row r="12" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="8">
         <v>107726</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="8">
         <v>106665</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="8">
         <v>105320</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="8">
         <v>104423</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="8">
         <v>103446</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="8">
         <v>102394</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="8">
         <v>98588</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="8">
         <v>98095</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="8">
         <v>98197</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="8">
         <v>98966</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="8">
         <v>101079</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="8">
         <v>103668</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="8">
         <v>104548</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="8">
         <v>104948</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="Q12" s="8">
         <v>104291</v>
       </c>
-      <c r="R12" s="14">
+      <c r="R12" s="8">
         <v>103866</v>
       </c>
       <c r="S12" s="15">
@@ -1207,56 +1266,56 @@
         <v>-0.16559798201528894</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="8">
         <v>121199</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="8">
         <v>120493</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="8">
         <v>120009</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="8">
         <v>120538</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="8">
         <v>121109</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="8">
         <v>121451</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="8">
         <v>120889</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="8">
         <v>121758</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="8">
         <v>122457</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="8">
         <v>123027</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="8">
         <v>124045</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="8">
         <v>123909</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="8">
         <v>123914</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="8">
         <v>124151</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13" s="8">
         <v>124371</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13" s="8">
         <v>123840</v>
       </c>
       <c r="S13" s="15">
@@ -1272,56 +1331,56 @@
         <v>8.8016795865633074E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="8">
         <v>175298</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="8">
         <v>174974</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="8">
         <v>174401</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="8">
         <v>173765</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="8">
         <v>173223</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="8">
         <v>172643</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="8">
         <v>170865</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="8">
         <v>171015</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="8">
         <v>171475</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="8">
         <v>172541</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="8">
         <v>174205</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="8">
         <v>174749</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="8">
         <v>175079</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="8">
         <v>175920</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="Q14" s="8">
         <v>176523</v>
       </c>
-      <c r="R14" s="14">
+      <c r="R14" s="8">
         <v>177227</v>
       </c>
       <c r="S14" s="15">
@@ -1337,56 +1396,56 @@
         <v>0.39045969293617788</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="8">
         <v>151452</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="8">
         <v>149656</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="8">
         <v>148091</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="8">
         <v>146187</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="8">
         <v>144680</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="8">
         <v>143014</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="8">
         <v>139575</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="8">
         <v>138655</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="8">
         <v>137833</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="8">
         <v>137256</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="8">
         <v>138236</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="8">
         <v>137979</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="8">
         <v>137563</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="8">
         <v>137014</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="Q15" s="8">
         <v>136292</v>
       </c>
-      <c r="R15" s="14">
+      <c r="R15" s="8">
         <v>134688</v>
       </c>
       <c r="S15" s="15">
@@ -1402,56 +1461,56 @@
         <v>-0.4736873366595391</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="8">
         <v>97749</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="8">
         <v>96972</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="8">
         <v>95871</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="8">
         <v>94870</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="8">
         <v>93903</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="8">
         <v>92836</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="8">
         <v>90919</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="8">
         <v>90391</v>
       </c>
-      <c r="K16" s="14">
+      <c r="K16" s="8">
         <v>90423</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="8">
         <v>90908</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="8">
         <v>91500</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="8">
         <v>92079</v>
       </c>
-      <c r="O16" s="14">
+      <c r="O16" s="8">
         <v>91720</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16" s="8">
         <v>91307</v>
       </c>
-      <c r="Q16" s="14">
+      <c r="Q16" s="8">
         <v>91297</v>
       </c>
-      <c r="R16" s="14">
+      <c r="R16" s="8">
         <v>91518</v>
       </c>
       <c r="S16" s="15">
@@ -1467,56 +1526,56 @@
         <v>-0.15188268974409405</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="8">
         <v>146690</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="8">
         <v>145488</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="8">
         <v>144044</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="8">
         <v>142321</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="8">
         <v>140553</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="8">
         <v>139060</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="8">
         <v>136516</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="8">
         <v>135418</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="8">
         <v>134661</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="8">
         <v>133905</v>
       </c>
-      <c r="M17" s="14">
+      <c r="M17" s="8">
         <v>134896</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17" s="8">
         <v>133610</v>
       </c>
-      <c r="O17" s="14">
+      <c r="O17" s="8">
         <v>133046</v>
       </c>
-      <c r="P17" s="14">
+      <c r="P17" s="8">
         <v>132765</v>
       </c>
-      <c r="Q17" s="14">
+      <c r="Q17" s="8">
         <v>132285</v>
       </c>
-      <c r="R17" s="14">
+      <c r="R17" s="8">
         <v>131772</v>
       </c>
       <c r="S17" s="15">
@@ -1532,56 +1591,56 @@
         <v>-5.3122059314573656E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="8">
         <v>134581</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="8">
         <v>134178</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="8">
         <v>133560</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="8">
         <v>132613</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="8">
         <v>132066</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="8">
         <v>131481</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="8">
         <v>130165</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="8">
         <v>130047</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="8">
         <v>130147</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="8">
         <v>130601</v>
       </c>
-      <c r="M18" s="14">
+      <c r="M18" s="8">
         <v>132320</v>
       </c>
-      <c r="N18" s="14">
+      <c r="N18" s="8">
         <v>132979</v>
       </c>
-      <c r="O18" s="14">
+      <c r="O18" s="8">
         <v>133368</v>
       </c>
-      <c r="P18" s="14">
+      <c r="P18" s="8">
         <v>133965</v>
       </c>
-      <c r="Q18" s="14">
+      <c r="Q18" s="8">
         <v>134801</v>
       </c>
-      <c r="R18" s="14">
+      <c r="R18" s="8">
         <v>135844</v>
       </c>
       <c r="S18" s="15">
@@ -1597,56 +1656,56 @@
         <v>0.82153057919378114</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="8">
         <v>126460</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="8">
         <v>125412</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="8">
         <v>124652</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="8">
         <v>123663</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="8">
         <v>122806</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="8">
         <v>122040</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="8">
         <v>120425</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="8">
         <v>120117</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="8">
         <v>119900</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="8">
         <v>120035</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19" s="8">
         <v>120981</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="8">
         <v>120904</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19" s="8">
         <v>120437</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19" s="8">
         <v>119960</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q19" s="8">
         <v>119622</v>
       </c>
-      <c r="R19" s="14">
+      <c r="R19" s="8">
         <v>119361</v>
       </c>
       <c r="S19" s="15">
@@ -1662,56 +1721,56 @@
         <v>-0.1147778587645881</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="8">
         <v>344905</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="8">
         <v>342767</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="8">
         <v>341759</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="8">
         <v>339828</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="8">
         <v>338162</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="8">
         <v>336372</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="8">
         <v>324550</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="8">
         <v>323311</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="8">
         <v>322427</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="8">
         <v>322509</v>
       </c>
-      <c r="M20" s="14">
+      <c r="M20" s="8">
         <v>325261</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20" s="8">
         <v>326244</v>
       </c>
-      <c r="O20" s="14">
+      <c r="O20" s="8">
         <v>327395</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20" s="8">
         <v>328074</v>
       </c>
-      <c r="Q20" s="14">
+      <c r="Q20" s="8">
         <v>326041</v>
       </c>
-      <c r="R20" s="14">
+      <c r="R20" s="8">
         <v>323900</v>
       </c>
       <c r="S20" s="15">
@@ -1727,121 +1786,121 @@
         <v>-7.3788206236492751E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="2:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="20">
         <v>1650435</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="20">
         <v>1641776</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="20">
         <v>1633318</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="20">
         <v>1623649</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="20">
         <v>1616720</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="20">
         <v>1609369</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="20">
         <v>1575968</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="20">
         <v>1574527</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="20">
         <v>1574936</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="20">
         <v>1579754</v>
       </c>
-      <c r="M21" s="14">
+      <c r="M21" s="20">
         <v>1598164</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="20">
         <v>1595609</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21" s="20">
         <v>1595734</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21" s="20">
         <v>1596396</v>
       </c>
-      <c r="Q21" s="14">
+      <c r="Q21" s="20">
         <v>1594929</v>
       </c>
-      <c r="R21" s="14">
+      <c r="R21" s="20">
         <v>1590577</v>
       </c>
-      <c r="S21" s="15">
+      <c r="S21" s="21">
         <v>1591424</v>
       </c>
-      <c r="T21" s="16">
+      <c r="T21" s="22">
         <v>-3.5754816154528957</v>
       </c>
-      <c r="U21" s="16">
+      <c r="U21" s="22">
         <v>-0.42173393969580092</v>
       </c>
-      <c r="V21" s="16">
+      <c r="V21" s="22">
         <v>5.3251115790056064E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+    <row r="22" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="8">
         <v>1128543</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="8">
         <v>1128772</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="8">
         <v>1130039</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="8">
         <v>1129797</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="8">
         <v>1130262</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="8">
         <v>1132130</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="8">
         <v>1106219</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="8">
         <v>1112675</v>
       </c>
-      <c r="K22" s="14">
+      <c r="K22" s="8">
         <v>1119526</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="8">
         <v>1128037</v>
       </c>
-      <c r="M22" s="14">
+      <c r="M22" s="8">
         <v>1144481</v>
       </c>
-      <c r="N22" s="14">
+      <c r="N22" s="8">
         <v>1148700</v>
       </c>
-      <c r="O22" s="14">
+      <c r="O22" s="8">
         <v>1152675</v>
       </c>
-      <c r="P22" s="14">
+      <c r="P22" s="8">
         <v>1157624</v>
       </c>
-      <c r="Q22" s="14">
+      <c r="Q22" s="8">
         <v>1157115</v>
       </c>
-      <c r="R22" s="14">
+      <c r="R22" s="8">
         <v>1155330</v>
       </c>
       <c r="S22" s="15">
@@ -1857,56 +1916,56 @@
         <v>0.19137389317337902</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+    <row r="23" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="8">
         <v>515729</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="8">
         <v>516343</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="8">
         <v>518069</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="8">
         <v>519619</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="8">
         <v>520966</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H23" s="8">
         <v>522686</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="8">
         <v>509485</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="8">
         <v>514137</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="8">
         <v>518386</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="8">
         <v>523642</v>
       </c>
-      <c r="M23" s="14">
+      <c r="M23" s="8">
         <v>532163</v>
       </c>
-      <c r="N23" s="14">
+      <c r="N23" s="8">
         <v>532864</v>
       </c>
-      <c r="O23" s="14">
+      <c r="O23" s="8">
         <v>535061</v>
       </c>
-      <c r="P23" s="14">
+      <c r="P23" s="8">
         <v>538068</v>
       </c>
-      <c r="Q23" s="14">
+      <c r="Q23" s="8">
         <v>536925</v>
       </c>
-      <c r="R23" s="14">
+      <c r="R23" s="8">
         <v>534049</v>
       </c>
       <c r="S23" s="15">
@@ -1922,56 +1981,56 @@
         <v>0.35258936914028488</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
+    <row r="24" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="8">
         <v>612814</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="8">
         <v>612429</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="8">
         <v>611970</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="8">
         <v>610178</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="8">
         <v>609296</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="8">
         <v>609444</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="8">
         <v>596734</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="8">
         <v>598538</v>
       </c>
-      <c r="K24" s="14">
+      <c r="K24" s="8">
         <v>601140</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="8">
         <v>604395</v>
       </c>
-      <c r="M24" s="14">
+      <c r="M24" s="8">
         <v>612318</v>
       </c>
-      <c r="N24" s="14">
+      <c r="N24" s="8">
         <v>615836</v>
       </c>
-      <c r="O24" s="14">
+      <c r="O24" s="8">
         <v>617614</v>
       </c>
-      <c r="P24" s="14">
+      <c r="P24" s="8">
         <v>619556</v>
       </c>
-      <c r="Q24" s="14">
+      <c r="Q24" s="8">
         <v>620190</v>
       </c>
-      <c r="R24" s="14">
+      <c r="R24" s="8">
         <v>621281</v>
       </c>
       <c r="S24" s="15">
@@ -1987,56 +2046,56 @@
         <v>5.2794146288072545E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
+    <row r="25" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="8">
         <v>215548</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="8">
         <v>215406</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="8">
         <v>215142</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="8">
         <v>214379</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="8">
         <v>213634</v>
       </c>
-      <c r="H25" s="14">
+      <c r="H25" s="8">
         <v>213558</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="8">
         <v>209745</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="8">
         <v>209671</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25" s="8">
         <v>209955</v>
       </c>
-      <c r="L25" s="14">
+      <c r="L25" s="8">
         <v>211093</v>
       </c>
-      <c r="M25" s="14">
+      <c r="M25" s="8">
         <v>213976</v>
       </c>
-      <c r="N25" s="14">
+      <c r="N25" s="8">
         <v>215082</v>
       </c>
-      <c r="O25" s="14">
+      <c r="O25" s="8">
         <v>216012</v>
       </c>
-      <c r="P25" s="14">
+      <c r="P25" s="8">
         <v>216886</v>
       </c>
-      <c r="Q25" s="14">
+      <c r="Q25" s="8">
         <v>217089</v>
       </c>
-      <c r="R25" s="14">
+      <c r="R25" s="8">
         <v>218072</v>
       </c>
       <c r="S25" s="15">
@@ -2052,56 +2111,56 @@
         <v>0.3517186984115338</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+    <row r="26" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="8">
         <v>159840</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="8">
         <v>158658</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="8">
         <v>157867</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="8">
         <v>156398</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="8">
         <v>155164</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="8">
         <v>154085</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="8">
         <v>149513</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="8">
         <v>148532</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K26" s="8">
         <v>147755</v>
       </c>
-      <c r="L26" s="14">
+      <c r="L26" s="8">
         <v>147813</v>
       </c>
-      <c r="M26" s="14">
+      <c r="M26" s="8">
         <v>148281</v>
       </c>
-      <c r="N26" s="14">
+      <c r="N26" s="8">
         <v>148265</v>
       </c>
-      <c r="O26" s="14">
+      <c r="O26" s="8">
         <v>148296</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26" s="8">
         <v>148559</v>
       </c>
-      <c r="Q26" s="14">
+      <c r="Q26" s="8">
         <v>148549</v>
       </c>
-      <c r="R26" s="14">
+      <c r="R26" s="8">
         <v>148580</v>
       </c>
       <c r="S26" s="15">
@@ -2117,56 +2176,56 @@
         <v>0.25777358998519317</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+    <row r="27" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="8">
         <v>290643</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="8">
         <v>289984</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="8">
         <v>288623</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="8">
         <v>286663</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="8">
         <v>284551</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="8">
         <v>282856</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="8">
         <v>276383</v>
       </c>
-      <c r="J27" s="14">
+      <c r="J27" s="8">
         <v>275330</v>
       </c>
-      <c r="K27" s="14">
+      <c r="K27" s="8">
         <v>274519</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="8">
         <v>274554</v>
       </c>
-      <c r="M27" s="14">
+      <c r="M27" s="8">
         <v>277055</v>
       </c>
-      <c r="N27" s="14">
+      <c r="N27" s="8">
         <v>277300</v>
       </c>
-      <c r="O27" s="14">
+      <c r="O27" s="8">
         <v>276640</v>
       </c>
-      <c r="P27" s="14">
+      <c r="P27" s="8">
         <v>276594</v>
       </c>
-      <c r="Q27" s="14">
+      <c r="Q27" s="8">
         <v>275817</v>
       </c>
-      <c r="R27" s="14">
+      <c r="R27" s="8">
         <v>275464</v>
       </c>
       <c r="S27" s="15">
@@ -2182,56 +2241,56 @@
         <v>-0.25084947579357014</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
+    <row r="28" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="8">
         <v>77918</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="8">
         <v>76888</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="8">
         <v>76103</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="8">
         <v>75092</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="8">
         <v>74094</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="8">
         <v>73240</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="8">
         <v>73155</v>
       </c>
-      <c r="J28" s="14">
+      <c r="J28" s="8">
         <v>72459</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K28" s="8">
         <v>71877</v>
       </c>
-      <c r="L28" s="14">
+      <c r="L28" s="8">
         <v>71438</v>
       </c>
-      <c r="M28" s="14">
+      <c r="M28" s="8">
         <v>71659</v>
       </c>
-      <c r="N28" s="14">
+      <c r="N28" s="8">
         <v>71510</v>
       </c>
-      <c r="O28" s="14">
+      <c r="O28" s="8">
         <v>71144</v>
       </c>
-      <c r="P28" s="14">
+      <c r="P28" s="8">
         <v>70975</v>
       </c>
-      <c r="Q28" s="14">
+      <c r="Q28" s="8">
         <v>70458</v>
       </c>
-      <c r="R28" s="14">
+      <c r="R28" s="8">
         <v>70207</v>
       </c>
       <c r="S28" s="15">
@@ -2247,56 +2306,56 @@
         <v>-0.49140399105502303</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+    <row r="29" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="8">
         <v>125870</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="8">
         <v>125436</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="8">
         <v>124895</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="8">
         <v>123881</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="8">
         <v>122989</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="8">
         <v>122206</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="8">
         <v>121390</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="8">
         <v>120225</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="8">
         <v>119848</v>
       </c>
-      <c r="L29" s="14">
+      <c r="L29" s="8">
         <v>119631</v>
       </c>
-      <c r="M29" s="14">
+      <c r="M29" s="8">
         <v>120632</v>
       </c>
-      <c r="N29" s="14">
+      <c r="N29" s="8">
         <v>121503</v>
       </c>
-      <c r="O29" s="14">
+      <c r="O29" s="8">
         <v>121470</v>
       </c>
-      <c r="P29" s="14">
+      <c r="P29" s="8">
         <v>121386</v>
       </c>
-      <c r="Q29" s="14">
+      <c r="Q29" s="8">
         <v>121390</v>
       </c>
-      <c r="R29" s="14">
+      <c r="R29" s="8">
         <v>121645</v>
       </c>
       <c r="S29" s="15">
@@ -2312,56 +2371,56 @@
         <v>0.10522421801142669</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="8">
         <v>165557</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="8">
         <v>165109</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="8">
         <v>164172</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="8">
         <v>162971</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="8">
         <v>161746</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="8">
         <v>160636</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="8">
         <v>157026</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="8">
         <v>156039</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="8">
         <v>155599</v>
       </c>
-      <c r="L30" s="14">
+      <c r="L30" s="8">
         <v>155847</v>
       </c>
-      <c r="M30" s="14">
+      <c r="M30" s="8">
         <v>156206</v>
       </c>
-      <c r="N30" s="14">
+      <c r="N30" s="8">
         <v>157616</v>
       </c>
-      <c r="O30" s="14">
+      <c r="O30" s="8">
         <v>157883</v>
       </c>
-      <c r="P30" s="14">
+      <c r="P30" s="8">
         <v>157781</v>
       </c>
-      <c r="Q30" s="14">
+      <c r="Q30" s="8">
         <v>157820</v>
       </c>
-      <c r="R30" s="14">
+      <c r="R30" s="8">
         <v>158406</v>
       </c>
       <c r="S30" s="15">
@@ -2377,121 +2436,121 @@
         <v>-0.18812418721513074</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="s">
+    <row r="31" spans="2:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="20">
         <v>2163919</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="20">
         <v>2160253</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="20">
         <v>2156841</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="20">
         <v>2149181</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="20">
         <v>2142440</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="20">
         <v>2138711</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="20">
         <v>2093431</v>
       </c>
-      <c r="J31" s="14">
+      <c r="J31" s="20">
         <v>2094931</v>
       </c>
-      <c r="K31" s="14">
+      <c r="K31" s="20">
         <v>2099079</v>
       </c>
-      <c r="L31" s="14">
+      <c r="L31" s="20">
         <v>2108413</v>
       </c>
-      <c r="M31" s="14">
+      <c r="M31" s="20">
         <v>2132290</v>
       </c>
-      <c r="N31" s="14">
+      <c r="N31" s="20">
         <v>2139976</v>
       </c>
-      <c r="O31" s="14">
+      <c r="O31" s="20">
         <v>2144120</v>
       </c>
-      <c r="P31" s="14">
+      <c r="P31" s="20">
         <v>2149805</v>
       </c>
-      <c r="Q31" s="14">
+      <c r="Q31" s="20">
         <v>2148238</v>
       </c>
-      <c r="R31" s="14">
+      <c r="R31" s="20">
         <v>2147704</v>
       </c>
-      <c r="S31" s="15">
+      <c r="S31" s="21">
         <v>2149859</v>
       </c>
-      <c r="T31" s="16">
+      <c r="T31" s="22">
         <v>-0.64974705615136241</v>
       </c>
-      <c r="U31" s="16">
+      <c r="U31" s="22">
         <v>0.82394983796763099</v>
       </c>
-      <c r="V31" s="16">
+      <c r="V31" s="22">
         <v>0.10033971161761583</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
+    <row r="32" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="8">
         <v>182444</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="8">
         <v>181936</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="8">
         <v>181115</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="8">
         <v>180130</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="8">
         <v>179247</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="8">
         <v>178528</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="8">
         <v>176054</v>
       </c>
-      <c r="J32" s="14">
+      <c r="J32" s="8">
         <v>175706</v>
       </c>
-      <c r="K32" s="14">
+      <c r="K32" s="8">
         <v>175552</v>
       </c>
-      <c r="L32" s="14">
+      <c r="L32" s="8">
         <v>176157</v>
       </c>
-      <c r="M32" s="14">
+      <c r="M32" s="8">
         <v>177971</v>
       </c>
-      <c r="N32" s="14">
+      <c r="N32" s="8">
         <v>178370</v>
       </c>
-      <c r="O32" s="14">
+      <c r="O32" s="8">
         <v>178764</v>
       </c>
-      <c r="P32" s="14">
+      <c r="P32" s="8">
         <v>178936</v>
       </c>
-      <c r="Q32" s="14">
+      <c r="Q32" s="8">
         <v>179011</v>
       </c>
-      <c r="R32" s="14">
+      <c r="R32" s="8">
         <v>179386</v>
       </c>
       <c r="S32" s="15">
@@ -2507,56 +2566,56 @@
         <v>0.29489480784453637</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
+    <row r="33" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="8">
         <v>205276</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="8">
         <v>204235</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="8">
         <v>202933</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="8">
         <v>202124</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="8">
         <v>201188</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="8">
         <v>200464</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="8">
         <v>198115</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="8">
         <v>197433</v>
       </c>
-      <c r="K33" s="14">
+      <c r="K33" s="8">
         <v>196607</v>
       </c>
-      <c r="L33" s="14">
+      <c r="L33" s="8">
         <v>196787</v>
       </c>
-      <c r="M33" s="14">
+      <c r="M33" s="8">
         <v>198103</v>
       </c>
-      <c r="N33" s="14">
+      <c r="N33" s="8">
         <v>198670</v>
       </c>
-      <c r="O33" s="14">
+      <c r="O33" s="8">
         <v>198100</v>
       </c>
-      <c r="P33" s="14">
+      <c r="P33" s="8">
         <v>198213</v>
       </c>
-      <c r="Q33" s="14">
+      <c r="Q33" s="8">
         <v>198038</v>
       </c>
-      <c r="R33" s="14">
+      <c r="R33" s="8">
         <v>198826</v>
       </c>
       <c r="S33" s="15">
@@ -2572,56 +2631,56 @@
         <v>0.39079396054841919</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
+    <row r="34" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="8">
         <v>241827</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="8">
         <v>242748</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="8">
         <v>243888</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="8">
         <v>244640</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="8">
         <v>245624</v>
       </c>
-      <c r="H34" s="14">
+      <c r="H34" s="8">
         <v>246868</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I34" s="8">
         <v>239269</v>
       </c>
-      <c r="J34" s="14">
+      <c r="J34" s="8">
         <v>240548</v>
       </c>
-      <c r="K34" s="14">
+      <c r="K34" s="8">
         <v>242871</v>
       </c>
-      <c r="L34" s="14">
+      <c r="L34" s="8">
         <v>245199</v>
       </c>
-      <c r="M34" s="14">
+      <c r="M34" s="8">
         <v>248122</v>
       </c>
-      <c r="N34" s="14">
+      <c r="N34" s="8">
         <v>250326</v>
       </c>
-      <c r="O34" s="14">
+      <c r="O34" s="8">
         <v>251511</v>
       </c>
-      <c r="P34" s="14">
+      <c r="P34" s="8">
         <v>252776</v>
       </c>
-      <c r="Q34" s="14">
+      <c r="Q34" s="8">
         <v>254431</v>
       </c>
-      <c r="R34" s="14">
+      <c r="R34" s="8">
         <v>256016</v>
       </c>
       <c r="S34" s="15">
@@ -2637,56 +2696,56 @@
         <v>0.59840009999375043</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
+    <row r="35" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="8">
         <v>51352</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="8">
         <v>50878</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="8">
         <v>50465</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="8">
         <v>49965</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="8">
         <v>49699</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H35" s="8">
         <v>49213</v>
       </c>
-      <c r="I35" s="14">
+      <c r="I35" s="8">
         <v>49082</v>
       </c>
-      <c r="J35" s="14">
+      <c r="J35" s="8">
         <v>48928</v>
       </c>
-      <c r="K35" s="14">
+      <c r="K35" s="8">
         <v>48670</v>
       </c>
-      <c r="L35" s="14">
+      <c r="L35" s="8">
         <v>48728</v>
       </c>
-      <c r="M35" s="14">
+      <c r="M35" s="8">
         <v>50128</v>
       </c>
-      <c r="N35" s="14">
+      <c r="N35" s="8">
         <v>48825</v>
       </c>
-      <c r="O35" s="14">
+      <c r="O35" s="8">
         <v>48357</v>
       </c>
-      <c r="P35" s="14">
+      <c r="P35" s="8">
         <v>48424</v>
       </c>
-      <c r="Q35" s="14">
+      <c r="Q35" s="8">
         <v>48412</v>
       </c>
-      <c r="R35" s="14">
+      <c r="R35" s="8">
         <v>48503</v>
       </c>
       <c r="S35" s="15">
@@ -2702,56 +2761,56 @@
         <v>-6.3913572356349091E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
+    <row r="36" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="8">
         <v>175441</v>
       </c>
-      <c r="D36" s="14">
+      <c r="D36" s="8">
         <v>175906</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="8">
         <v>176445</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="8">
         <v>176512</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="8">
         <v>177042</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="8">
         <v>177279</v>
       </c>
-      <c r="I36" s="14">
+      <c r="I36" s="8">
         <v>174685</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="8">
         <v>175640</v>
       </c>
-      <c r="K36" s="14">
+      <c r="K36" s="8">
         <v>176727</v>
       </c>
-      <c r="L36" s="14">
+      <c r="L36" s="8">
         <v>178122</v>
       </c>
-      <c r="M36" s="14">
+      <c r="M36" s="8">
         <v>180719</v>
       </c>
-      <c r="N36" s="14">
+      <c r="N36" s="8">
         <v>181605</v>
       </c>
-      <c r="O36" s="14">
+      <c r="O36" s="8">
         <v>182930</v>
       </c>
-      <c r="P36" s="14">
+      <c r="P36" s="8">
         <v>183372</v>
       </c>
-      <c r="Q36" s="14">
+      <c r="Q36" s="8">
         <v>184139</v>
       </c>
-      <c r="R36" s="14">
+      <c r="R36" s="8">
         <v>184235</v>
       </c>
       <c r="S36" s="15">
@@ -2767,56 +2826,56 @@
         <v>0.48524981681005236</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="13" t="s">
+    <row r="37" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="8">
         <v>112741</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="8">
         <v>112498</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="8">
         <v>112679</v>
       </c>
-      <c r="F37" s="14">
+      <c r="F37" s="8">
         <v>112486</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="8">
         <v>112029</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H37" s="8">
         <v>111876</v>
       </c>
-      <c r="I37" s="14">
+      <c r="I37" s="8">
         <v>110842</v>
       </c>
-      <c r="J37" s="14">
+      <c r="J37" s="8">
         <v>110816</v>
       </c>
-      <c r="K37" s="14">
+      <c r="K37" s="8">
         <v>110882</v>
       </c>
-      <c r="L37" s="14">
+      <c r="L37" s="8">
         <v>111484</v>
       </c>
-      <c r="M37" s="14">
+      <c r="M37" s="8">
         <v>113579</v>
       </c>
-      <c r="N37" s="14">
+      <c r="N37" s="8">
         <v>112695</v>
       </c>
-      <c r="O37" s="14">
+      <c r="O37" s="8">
         <v>113105</v>
       </c>
-      <c r="P37" s="14">
+      <c r="P37" s="8">
         <v>113517</v>
       </c>
-      <c r="Q37" s="14">
+      <c r="Q37" s="8">
         <v>113928</v>
       </c>
-      <c r="R37" s="14">
+      <c r="R37" s="8">
         <v>114640</v>
       </c>
       <c r="S37" s="15">
@@ -2832,56 +2891,56 @@
         <v>0.3611304954640614</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+    <row r="38" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="8">
         <v>164875</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="8">
         <v>164958</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="8">
         <v>165074</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="8">
         <v>164603</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="8">
         <v>164064</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="8">
         <v>163860</v>
       </c>
-      <c r="I38" s="14">
+      <c r="I38" s="8">
         <v>162182</v>
       </c>
-      <c r="J38" s="14">
+      <c r="J38" s="8">
         <v>161780</v>
       </c>
-      <c r="K38" s="14">
+      <c r="K38" s="8">
         <v>161308</v>
       </c>
-      <c r="L38" s="14">
+      <c r="L38" s="8">
         <v>161842</v>
       </c>
-      <c r="M38" s="14">
+      <c r="M38" s="8">
         <v>163253</v>
       </c>
-      <c r="N38" s="14">
+      <c r="N38" s="8">
         <v>163372</v>
       </c>
-      <c r="O38" s="14">
+      <c r="O38" s="8">
         <v>163377</v>
       </c>
-      <c r="P38" s="14">
+      <c r="P38" s="8">
         <v>163455</v>
       </c>
-      <c r="Q38" s="14">
+      <c r="Q38" s="8">
         <v>163782</v>
       </c>
-      <c r="R38" s="14">
+      <c r="R38" s="8">
         <v>164486</v>
       </c>
       <c r="S38" s="15">
@@ -2897,56 +2956,56 @@
         <v>0.31309655532993691</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
+    <row r="39" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="8">
         <v>142678</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="8">
         <v>142234</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="8">
         <v>141692</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="8">
         <v>140792</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="8">
         <v>140053</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="8">
         <v>139630</v>
       </c>
-      <c r="I39" s="14">
+      <c r="I39" s="8">
         <v>136072</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="8">
         <v>135772</v>
       </c>
-      <c r="K39" s="14">
+      <c r="K39" s="8">
         <v>136251</v>
       </c>
-      <c r="L39" s="14">
+      <c r="L39" s="8">
         <v>136200</v>
       </c>
-      <c r="M39" s="14">
+      <c r="M39" s="8">
         <v>140264</v>
       </c>
-      <c r="N39" s="14">
+      <c r="N39" s="8">
         <v>139641</v>
       </c>
-      <c r="O39" s="14">
+      <c r="O39" s="8">
         <v>139099</v>
       </c>
-      <c r="P39" s="14">
+      <c r="P39" s="8">
         <v>139755</v>
       </c>
-      <c r="Q39" s="14">
+      <c r="Q39" s="8">
         <v>140673</v>
       </c>
-      <c r="R39" s="14">
+      <c r="R39" s="8">
         <v>140885</v>
       </c>
       <c r="S39" s="15">
@@ -2962,56 +3021,56 @@
         <v>1.438762110941548</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B40" s="13" t="s">
+    <row r="40" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="8">
         <v>196475</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="8">
         <v>197122</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="8">
         <v>197091</v>
       </c>
-      <c r="F40" s="14">
+      <c r="F40" s="8">
         <v>196891</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="8">
         <v>196952</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="8">
         <v>197132</v>
       </c>
-      <c r="I40" s="14">
+      <c r="I40" s="8">
         <v>195606</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40" s="8">
         <v>195779</v>
       </c>
-      <c r="K40" s="14">
+      <c r="K40" s="8">
         <v>196516</v>
       </c>
-      <c r="L40" s="14">
+      <c r="L40" s="8">
         <v>197448</v>
       </c>
-      <c r="M40" s="14">
+      <c r="M40" s="8">
         <v>200054</v>
       </c>
-      <c r="N40" s="14">
+      <c r="N40" s="8">
         <v>201638</v>
       </c>
-      <c r="O40" s="14">
+      <c r="O40" s="8">
         <v>201887</v>
       </c>
-      <c r="P40" s="14">
+      <c r="P40" s="8">
         <v>203102</v>
       </c>
-      <c r="Q40" s="14">
+      <c r="Q40" s="8">
         <v>204512</v>
       </c>
-      <c r="R40" s="14">
+      <c r="R40" s="8">
         <v>205357</v>
       </c>
       <c r="S40" s="15">
@@ -3027,56 +3086,56 @@
         <v>0.55464386410007938</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="13" t="s">
+    <row r="41" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="8">
         <v>96940</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="8">
         <v>96458</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="8">
         <v>95983</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="8">
         <v>94940</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="8">
         <v>94428</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="8">
         <v>94020</v>
       </c>
-      <c r="I41" s="14">
+      <c r="I41" s="8">
         <v>93284</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41" s="8">
         <v>92801</v>
       </c>
-      <c r="K41" s="14">
+      <c r="K41" s="8">
         <v>92356</v>
       </c>
-      <c r="L41" s="14">
+      <c r="L41" s="8">
         <v>92533</v>
       </c>
-      <c r="M41" s="14">
+      <c r="M41" s="8">
         <v>93131</v>
       </c>
-      <c r="N41" s="14">
+      <c r="N41" s="8">
         <v>92961</v>
       </c>
-      <c r="O41" s="14">
+      <c r="O41" s="8">
         <v>92744</v>
       </c>
-      <c r="P41" s="14">
+      <c r="P41" s="8">
         <v>92572</v>
       </c>
-      <c r="Q41" s="14">
+      <c r="Q41" s="8">
         <v>92389</v>
       </c>
-      <c r="R41" s="14">
+      <c r="R41" s="8">
         <v>92566</v>
       </c>
       <c r="S41" s="15">
@@ -3092,56 +3151,56 @@
         <v>0.35434176695546959</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="13" t="s">
+    <row r="42" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="8">
         <v>134084</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D42" s="8">
         <v>133965</v>
       </c>
-      <c r="E42" s="14">
+      <c r="E42" s="8">
         <v>133767</v>
       </c>
-      <c r="F42" s="14">
+      <c r="F42" s="8">
         <v>133560</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="8">
         <v>133328</v>
       </c>
-      <c r="H42" s="14">
+      <c r="H42" s="8">
         <v>133368</v>
       </c>
-      <c r="I42" s="14">
+      <c r="I42" s="8">
         <v>131936</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="8">
         <v>132129</v>
       </c>
-      <c r="K42" s="14">
+      <c r="K42" s="8">
         <v>132459</v>
       </c>
-      <c r="L42" s="14">
+      <c r="L42" s="8">
         <v>133215</v>
       </c>
-      <c r="M42" s="14">
+      <c r="M42" s="8">
         <v>134645</v>
       </c>
-      <c r="N42" s="14">
+      <c r="N42" s="8">
         <v>135842</v>
       </c>
-      <c r="O42" s="14">
+      <c r="O42" s="8">
         <v>136590</v>
       </c>
-      <c r="P42" s="14">
+      <c r="P42" s="8">
         <v>136792</v>
       </c>
-      <c r="Q42" s="14">
+      <c r="Q42" s="8">
         <v>137133</v>
       </c>
-      <c r="R42" s="14">
+      <c r="R42" s="8">
         <v>137574</v>
       </c>
       <c r="S42" s="15">
@@ -3157,121 +3216,121 @@
         <v>0.67818047014697547</v>
       </c>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
+    <row r="43" spans="2:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="20">
         <v>1704133</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="20">
         <v>1702938</v>
       </c>
-      <c r="E43" s="14">
+      <c r="E43" s="20">
         <v>1701132</v>
       </c>
-      <c r="F43" s="14">
+      <c r="F43" s="20">
         <v>1696643</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="20">
         <v>1693654</v>
       </c>
-      <c r="H43" s="14">
+      <c r="H43" s="20">
         <v>1692238</v>
       </c>
-      <c r="I43" s="14">
+      <c r="I43" s="20">
         <v>1667127</v>
       </c>
-      <c r="J43" s="14">
+      <c r="J43" s="20">
         <v>1667332</v>
       </c>
-      <c r="K43" s="14">
+      <c r="K43" s="20">
         <v>1670199</v>
       </c>
-      <c r="L43" s="14">
+      <c r="L43" s="20">
         <v>1677715</v>
       </c>
-      <c r="M43" s="14">
+      <c r="M43" s="20">
         <v>1699969</v>
       </c>
-      <c r="N43" s="14">
+      <c r="N43" s="20">
         <v>1703945</v>
       </c>
-      <c r="O43" s="14">
+      <c r="O43" s="20">
         <v>1706464</v>
       </c>
-      <c r="P43" s="14">
+      <c r="P43" s="20">
         <v>1710914</v>
       </c>
-      <c r="Q43" s="14">
+      <c r="Q43" s="20">
         <v>1716448</v>
       </c>
-      <c r="R43" s="14">
+      <c r="R43" s="20">
         <v>1722474</v>
       </c>
-      <c r="S43" s="15">
+      <c r="S43" s="21">
         <v>1731531</v>
       </c>
-      <c r="T43" s="16">
+      <c r="T43" s="22">
         <v>1.6077383631441913</v>
       </c>
-      <c r="U43" s="16">
+      <c r="U43" s="22">
         <v>1.8566220913440186</v>
       </c>
-      <c r="V43" s="16">
+      <c r="V43" s="22">
         <v>0.52581345204630081</v>
       </c>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="13" t="s">
+    <row r="44" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="8">
         <v>75916</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="8">
         <v>75320</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E44" s="8">
         <v>75135</v>
       </c>
-      <c r="F44" s="14">
+      <c r="F44" s="8">
         <v>74751</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="8">
         <v>74512</v>
       </c>
-      <c r="H44" s="14">
+      <c r="H44" s="8">
         <v>74361</v>
       </c>
-      <c r="I44" s="14">
+      <c r="I44" s="8">
         <v>73364</v>
       </c>
-      <c r="J44" s="14">
+      <c r="J44" s="8">
         <v>73588</v>
       </c>
-      <c r="K44" s="14">
+      <c r="K44" s="8">
         <v>74052</v>
       </c>
-      <c r="L44" s="14">
+      <c r="L44" s="8">
         <v>74804</v>
       </c>
-      <c r="M44" s="14">
+      <c r="M44" s="8">
         <v>76323</v>
       </c>
-      <c r="N44" s="14">
+      <c r="N44" s="8">
         <v>77045</v>
       </c>
-      <c r="O44" s="14">
+      <c r="O44" s="8">
         <v>77521</v>
       </c>
-      <c r="P44" s="14">
+      <c r="P44" s="8">
         <v>77607</v>
       </c>
-      <c r="Q44" s="14">
+      <c r="Q44" s="8">
         <v>77559</v>
       </c>
-      <c r="R44" s="14">
+      <c r="R44" s="8">
         <v>77503</v>
       </c>
       <c r="S44" s="15">
@@ -3287,56 +3346,56 @@
         <v>2.451518005754616E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="13" t="s">
+    <row r="45" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="8">
         <v>51693</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="8">
         <v>51742</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="8">
         <v>51714</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="8">
         <v>51562</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="8">
         <v>51292</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45" s="8">
         <v>51616</v>
       </c>
-      <c r="I45" s="14">
+      <c r="I45" s="8">
         <v>49848</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="8">
         <v>49751</v>
       </c>
-      <c r="K45" s="14">
+      <c r="K45" s="8">
         <v>49790</v>
       </c>
-      <c r="L45" s="14">
+      <c r="L45" s="8">
         <v>50016</v>
       </c>
-      <c r="M45" s="14">
+      <c r="M45" s="8">
         <v>50694</v>
       </c>
-      <c r="N45" s="14">
+      <c r="N45" s="8">
         <v>50486</v>
       </c>
-      <c r="O45" s="14">
+      <c r="O45" s="8">
         <v>50607</v>
       </c>
-      <c r="P45" s="14">
+      <c r="P45" s="8">
         <v>50195</v>
       </c>
-      <c r="Q45" s="14">
+      <c r="Q45" s="8">
         <v>49913</v>
       </c>
-      <c r="R45" s="14">
+      <c r="R45" s="8">
         <v>49874</v>
       </c>
       <c r="S45" s="15">
@@ -3352,56 +3411,56 @@
         <v>-0.70377350924329307</v>
       </c>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="13" t="s">
+    <row r="46" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="8">
         <v>158565</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="8">
         <v>159060</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="8">
         <v>159563</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F46" s="8">
         <v>160279</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G46" s="8">
         <v>161334</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H46" s="8">
         <v>162173</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I46" s="8">
         <v>157706</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="8">
         <v>158658</v>
       </c>
-      <c r="K46" s="14">
+      <c r="K46" s="8">
         <v>159610</v>
       </c>
-      <c r="L46" s="14">
+      <c r="L46" s="8">
         <v>160907</v>
       </c>
-      <c r="M46" s="14">
+      <c r="M46" s="8">
         <v>163830</v>
       </c>
-      <c r="N46" s="14">
+      <c r="N46" s="8">
         <v>165711</v>
       </c>
-      <c r="O46" s="14">
+      <c r="O46" s="8">
         <v>167081</v>
       </c>
-      <c r="P46" s="14">
+      <c r="P46" s="8">
         <v>168210</v>
       </c>
-      <c r="Q46" s="14">
+      <c r="Q46" s="8">
         <v>169077</v>
       </c>
-      <c r="R46" s="14">
+      <c r="R46" s="8">
         <v>169605</v>
       </c>
       <c r="S46" s="15">
@@ -3417,56 +3476,56 @@
         <v>0.46225052327466759</v>
       </c>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="13" t="s">
+    <row r="47" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="8">
         <v>163814</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="8">
         <v>163020</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="8">
         <v>162870</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="8">
         <v>163286</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="8">
         <v>163514</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="8">
         <v>164119</v>
       </c>
-      <c r="I47" s="14">
+      <c r="I47" s="8">
         <v>154513</v>
       </c>
-      <c r="J47" s="14">
+      <c r="J47" s="8">
         <v>155625</v>
       </c>
-      <c r="K47" s="14">
+      <c r="K47" s="8">
         <v>156315</v>
       </c>
-      <c r="L47" s="14">
+      <c r="L47" s="8">
         <v>156897</v>
       </c>
-      <c r="M47" s="14">
+      <c r="M47" s="8">
         <v>162403</v>
       </c>
-      <c r="N47" s="14">
+      <c r="N47" s="8">
         <v>164070</v>
       </c>
-      <c r="O47" s="14">
+      <c r="O47" s="8">
         <v>164374</v>
       </c>
-      <c r="P47" s="14">
+      <c r="P47" s="8">
         <v>164748</v>
       </c>
-      <c r="Q47" s="14">
+      <c r="Q47" s="8">
         <v>165251</v>
       </c>
-      <c r="R47" s="14">
+      <c r="R47" s="8">
         <v>164223</v>
       </c>
       <c r="S47" s="15">
@@ -3482,56 +3541,56 @@
         <v>0.49384069222946847</v>
       </c>
     </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B48" s="13" t="s">
+    <row r="48" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="8">
         <v>83552</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="8">
         <v>82797</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="8">
         <v>82192</v>
       </c>
-      <c r="F48" s="14">
+      <c r="F48" s="8">
         <v>81411</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G48" s="8">
         <v>81137</v>
       </c>
-      <c r="H48" s="14">
+      <c r="H48" s="8">
         <v>81324</v>
       </c>
-      <c r="I48" s="14">
+      <c r="I48" s="8">
         <v>76926</v>
       </c>
-      <c r="J48" s="14">
+      <c r="J48" s="8">
         <v>76545</v>
       </c>
-      <c r="K48" s="14">
+      <c r="K48" s="8">
         <v>75728</v>
       </c>
-      <c r="L48" s="14">
+      <c r="L48" s="8">
         <v>75534</v>
       </c>
-      <c r="M48" s="14">
+      <c r="M48" s="8">
         <v>75995</v>
       </c>
-      <c r="N48" s="14">
+      <c r="N48" s="8">
         <v>76201</v>
       </c>
-      <c r="O48" s="14">
+      <c r="O48" s="8">
         <v>76316</v>
       </c>
-      <c r="P48" s="14">
+      <c r="P48" s="8">
         <v>76278</v>
       </c>
-      <c r="Q48" s="14">
+      <c r="Q48" s="8">
         <v>76089</v>
       </c>
-      <c r="R48" s="14">
+      <c r="R48" s="8">
         <v>75189</v>
       </c>
       <c r="S48" s="15">
@@ -3547,56 +3606,56 @@
         <v>-0.21545704823843914</v>
       </c>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B49" s="13" t="s">
+    <row r="49" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="8">
         <v>115891</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="8">
         <v>116626</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="8">
         <v>117041</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="8">
         <v>117102</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="8">
         <v>117517</v>
       </c>
-      <c r="H49" s="14">
+      <c r="H49" s="8">
         <v>118004</v>
       </c>
-      <c r="I49" s="14">
+      <c r="I49" s="8">
         <v>117951</v>
       </c>
-      <c r="J49" s="14">
+      <c r="J49" s="8">
         <v>118489</v>
       </c>
-      <c r="K49" s="14">
+      <c r="K49" s="8">
         <v>118865</v>
       </c>
-      <c r="L49" s="14">
+      <c r="L49" s="8">
         <v>119917</v>
       </c>
-      <c r="M49" s="14">
+      <c r="M49" s="8">
         <v>121435</v>
       </c>
-      <c r="N49" s="14">
+      <c r="N49" s="8">
         <v>122698</v>
       </c>
-      <c r="O49" s="14">
+      <c r="O49" s="8">
         <v>123377</v>
       </c>
-      <c r="P49" s="14">
+      <c r="P49" s="8">
         <v>124071</v>
       </c>
-      <c r="Q49" s="14">
+      <c r="Q49" s="8">
         <v>124859</v>
       </c>
-      <c r="R49" s="14">
+      <c r="R49" s="8">
         <v>125643</v>
       </c>
       <c r="S49" s="15">
@@ -3612,56 +3671,56 @@
         <v>0.66219367573203447</v>
       </c>
     </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
+    <row r="50" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="14">
+      <c r="C50" s="8">
         <v>190128</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50" s="8">
         <v>190252</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50" s="8">
         <v>190293</v>
       </c>
-      <c r="F50" s="14">
+      <c r="F50" s="8">
         <v>189381</v>
       </c>
-      <c r="G50" s="14">
+      <c r="G50" s="8">
         <v>188973</v>
       </c>
-      <c r="H50" s="14">
+      <c r="H50" s="8">
         <v>188947</v>
       </c>
-      <c r="I50" s="14">
+      <c r="I50" s="8">
         <v>186713</v>
       </c>
-      <c r="J50" s="14">
+      <c r="J50" s="8">
         <v>186673</v>
       </c>
-      <c r="K50" s="14">
+      <c r="K50" s="8">
         <v>187058</v>
       </c>
-      <c r="L50" s="14">
+      <c r="L50" s="8">
         <v>187998</v>
       </c>
-      <c r="M50" s="14">
+      <c r="M50" s="8">
         <v>189199</v>
       </c>
-      <c r="N50" s="14">
+      <c r="N50" s="8">
         <v>190066</v>
       </c>
-      <c r="O50" s="14">
+      <c r="O50" s="8">
         <v>189949</v>
       </c>
-      <c r="P50" s="14">
+      <c r="P50" s="8">
         <v>189848</v>
       </c>
-      <c r="Q50" s="14">
+      <c r="Q50" s="8">
         <v>189694</v>
       </c>
-      <c r="R50" s="14">
+      <c r="R50" s="8">
         <v>190178</v>
       </c>
       <c r="S50" s="15">
@@ -3677,56 +3736,56 @@
         <v>0.12987832451703141</v>
       </c>
     </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B51" s="13" t="s">
+    <row r="51" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="8">
         <v>155642</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51" s="8">
         <v>156241</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="8">
         <v>157164</v>
       </c>
-      <c r="F51" s="14">
+      <c r="F51" s="8">
         <v>157268</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G51" s="8">
         <v>157506</v>
       </c>
-      <c r="H51" s="14">
+      <c r="H51" s="8">
         <v>158194</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I51" s="8">
         <v>159290</v>
       </c>
-      <c r="J51" s="14">
+      <c r="J51" s="8">
         <v>160033</v>
       </c>
-      <c r="K51" s="14">
+      <c r="K51" s="8">
         <v>160176</v>
       </c>
-      <c r="L51" s="14">
+      <c r="L51" s="8">
         <v>162350</v>
       </c>
-      <c r="M51" s="14">
+      <c r="M51" s="8">
         <v>164734</v>
       </c>
-      <c r="N51" s="14">
+      <c r="N51" s="8">
         <v>165930</v>
       </c>
-      <c r="O51" s="14">
+      <c r="O51" s="8">
         <v>167925</v>
       </c>
-      <c r="P51" s="14">
+      <c r="P51" s="8">
         <v>169348</v>
       </c>
-      <c r="Q51" s="14">
+      <c r="Q51" s="8">
         <v>170682</v>
       </c>
-      <c r="R51" s="14">
+      <c r="R51" s="8">
         <v>172632</v>
       </c>
       <c r="S51" s="15">
@@ -3742,56 +3801,56 @@
         <v>0.7808517540201122</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B52" s="13" t="s">
+    <row r="52" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52" s="8">
         <v>310088</v>
       </c>
-      <c r="D52" s="14">
+      <c r="D52" s="8">
         <v>311965</v>
       </c>
-      <c r="E52" s="14">
+      <c r="E52" s="8">
         <v>313533</v>
       </c>
-      <c r="F52" s="14">
+      <c r="F52" s="8">
         <v>313824</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G52" s="8">
         <v>313098</v>
       </c>
-      <c r="H52" s="14">
+      <c r="H52" s="8">
         <v>313056</v>
       </c>
-      <c r="I52" s="14">
+      <c r="I52" s="8">
         <v>311634</v>
       </c>
-      <c r="J52" s="14">
+      <c r="J52" s="8">
         <v>312855</v>
       </c>
-      <c r="K52" s="14">
+      <c r="K52" s="8">
         <v>313689</v>
       </c>
-      <c r="L52" s="14">
+      <c r="L52" s="8">
         <v>315757</v>
       </c>
-      <c r="M52" s="14">
+      <c r="M52" s="8">
         <v>319488</v>
       </c>
-      <c r="N52" s="14">
+      <c r="N52" s="8">
         <v>321391</v>
       </c>
-      <c r="O52" s="14">
+      <c r="O52" s="8">
         <v>323636</v>
       </c>
-      <c r="P52" s="14">
+      <c r="P52" s="8">
         <v>325657</v>
       </c>
-      <c r="Q52" s="14">
+      <c r="Q52" s="8">
         <v>326954</v>
       </c>
-      <c r="R52" s="14">
+      <c r="R52" s="8">
         <v>328930</v>
       </c>
       <c r="S52" s="15">
@@ -3807,56 +3866,56 @@
         <v>0.75000760040130121</v>
       </c>
     </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B53" s="13" t="s">
+    <row r="53" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="8">
         <v>101412</v>
       </c>
-      <c r="D53" s="14">
+      <c r="D53" s="8">
         <v>101192</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E53" s="8">
         <v>100779</v>
       </c>
-      <c r="F53" s="14">
+      <c r="F53" s="8">
         <v>100307</v>
       </c>
-      <c r="G53" s="14">
+      <c r="G53" s="8">
         <v>99851</v>
       </c>
-      <c r="H53" s="14">
+      <c r="H53" s="8">
         <v>99598</v>
       </c>
-      <c r="I53" s="14">
+      <c r="I53" s="8">
         <v>97857</v>
       </c>
-      <c r="J53" s="14">
+      <c r="J53" s="8">
         <v>97327</v>
       </c>
-      <c r="K53" s="14">
+      <c r="K53" s="8">
         <v>97093</v>
       </c>
-      <c r="L53" s="14">
+      <c r="L53" s="8">
         <v>96937</v>
       </c>
-      <c r="M53" s="14">
+      <c r="M53" s="8">
         <v>97900</v>
       </c>
-      <c r="N53" s="14">
+      <c r="N53" s="8">
         <v>98409</v>
       </c>
-      <c r="O53" s="14">
+      <c r="O53" s="8">
         <v>98509</v>
       </c>
-      <c r="P53" s="14">
+      <c r="P53" s="8">
         <v>98460</v>
       </c>
-      <c r="Q53" s="14">
+      <c r="Q53" s="8">
         <v>98704</v>
       </c>
-      <c r="R53" s="14">
+      <c r="R53" s="8">
         <v>98971</v>
       </c>
       <c r="S53" s="15">
@@ -3872,56 +3931,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
+    <row r="54" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="8">
         <v>134442</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="8">
         <v>134840</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="8">
         <v>135270</v>
       </c>
-      <c r="F54" s="14">
+      <c r="F54" s="8">
         <v>135508</v>
       </c>
-      <c r="G54" s="14">
+      <c r="G54" s="8">
         <v>135346</v>
       </c>
-      <c r="H54" s="14">
+      <c r="H54" s="8">
         <v>135047</v>
       </c>
-      <c r="I54" s="14">
+      <c r="I54" s="8">
         <v>133400</v>
       </c>
-      <c r="J54" s="14">
+      <c r="J54" s="8">
         <v>133652</v>
       </c>
-      <c r="K54" s="14">
+      <c r="K54" s="8">
         <v>133678</v>
       </c>
-      <c r="L54" s="14">
+      <c r="L54" s="8">
         <v>134329</v>
       </c>
-      <c r="M54" s="14">
+      <c r="M54" s="8">
         <v>135662</v>
       </c>
-      <c r="N54" s="14">
+      <c r="N54" s="8">
         <v>135770</v>
       </c>
-      <c r="O54" s="14">
+      <c r="O54" s="8">
         <v>135859</v>
       </c>
-      <c r="P54" s="14">
+      <c r="P54" s="8">
         <v>136511</v>
       </c>
-      <c r="Q54" s="14">
+      <c r="Q54" s="8">
         <v>137162</v>
       </c>
-      <c r="R54" s="14">
+      <c r="R54" s="8">
         <v>137891</v>
       </c>
       <c r="S54" s="15">
@@ -3937,56 +3996,56 @@
         <v>0.6026499191390301</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B55" s="13" t="s">
+    <row r="55" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="8">
         <v>165056</v>
       </c>
-      <c r="D55" s="14">
+      <c r="D55" s="8">
         <v>165347</v>
       </c>
-      <c r="E55" s="14">
+      <c r="E55" s="8">
         <v>165088</v>
       </c>
-      <c r="F55" s="14">
+      <c r="F55" s="8">
         <v>164947</v>
       </c>
-      <c r="G55" s="14">
+      <c r="G55" s="8">
         <v>164837</v>
       </c>
-      <c r="H55" s="14">
+      <c r="H55" s="8">
         <v>164705</v>
       </c>
-      <c r="I55" s="14">
+      <c r="I55" s="8">
         <v>163991</v>
       </c>
-      <c r="J55" s="14">
+      <c r="J55" s="8">
         <v>164202</v>
       </c>
-      <c r="K55" s="14">
+      <c r="K55" s="8">
         <v>164792</v>
       </c>
-      <c r="L55" s="14">
+      <c r="L55" s="8">
         <v>165809</v>
       </c>
-      <c r="M55" s="14">
+      <c r="M55" s="8">
         <v>167548</v>
       </c>
-      <c r="N55" s="14">
+      <c r="N55" s="8">
         <v>168253</v>
       </c>
-      <c r="O55" s="14">
+      <c r="O55" s="8">
         <v>168946</v>
       </c>
-      <c r="P55" s="14">
+      <c r="P55" s="8">
         <v>169809</v>
       </c>
-      <c r="Q55" s="14">
+      <c r="Q55" s="8">
         <v>170756</v>
       </c>
-      <c r="R55" s="14">
+      <c r="R55" s="8">
         <v>171483</v>
       </c>
       <c r="S55" s="15">
@@ -4002,56 +4061,56 @@
         <v>0.54699299639031274</v>
       </c>
     </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B56" s="13" t="s">
+    <row r="56" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="8">
         <v>125731</v>
       </c>
-      <c r="D56" s="14">
+      <c r="D56" s="8">
         <v>125949</v>
       </c>
-      <c r="E56" s="14">
+      <c r="E56" s="8">
         <v>126131</v>
       </c>
-      <c r="F56" s="14">
+      <c r="F56" s="8">
         <v>125943</v>
       </c>
-      <c r="G56" s="14">
+      <c r="G56" s="8">
         <v>126571</v>
       </c>
-      <c r="H56" s="14">
+      <c r="H56" s="8">
         <v>127282</v>
       </c>
-      <c r="I56" s="14">
+      <c r="I56" s="8">
         <v>125265</v>
       </c>
-      <c r="J56" s="14">
+      <c r="J56" s="8">
         <v>125413</v>
       </c>
-      <c r="K56" s="14">
+      <c r="K56" s="8">
         <v>125778</v>
       </c>
-      <c r="L56" s="14">
+      <c r="L56" s="8">
         <v>126798</v>
       </c>
-      <c r="M56" s="14">
+      <c r="M56" s="8">
         <v>128608</v>
       </c>
-      <c r="N56" s="14">
+      <c r="N56" s="8">
         <v>129484</v>
       </c>
-      <c r="O56" s="14">
+      <c r="O56" s="8">
         <v>129924</v>
       </c>
-      <c r="P56" s="14">
+      <c r="P56" s="8">
         <v>130144</v>
       </c>
-      <c r="Q56" s="14">
+      <c r="Q56" s="8">
         <v>130890</v>
       </c>
-      <c r="R56" s="14">
+      <c r="R56" s="8">
         <v>131467</v>
       </c>
       <c r="S56" s="15">
@@ -4067,56 +4126,56 @@
         <v>0.47464382696798435</v>
       </c>
     </row>
-    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B57" s="13" t="s">
+    <row r="57" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="8">
         <v>359449</v>
       </c>
-      <c r="D57" s="14">
+      <c r="D57" s="8">
         <v>359340</v>
       </c>
-      <c r="E57" s="14">
+      <c r="E57" s="8">
         <v>358852</v>
       </c>
-      <c r="F57" s="14">
+      <c r="F57" s="8">
         <v>358236</v>
       </c>
-      <c r="G57" s="14">
+      <c r="G57" s="8">
         <v>357056</v>
       </c>
-      <c r="H57" s="14">
+      <c r="H57" s="8">
         <v>356123</v>
       </c>
-      <c r="I57" s="14">
+      <c r="I57" s="8">
         <v>350418</v>
       </c>
-      <c r="J57" s="14">
+      <c r="J57" s="8">
         <v>350444</v>
       </c>
-      <c r="K57" s="14">
+      <c r="K57" s="8">
         <v>350302</v>
       </c>
-      <c r="L57" s="14">
+      <c r="L57" s="8">
         <v>351316</v>
       </c>
-      <c r="M57" s="14">
+      <c r="M57" s="8">
         <v>358079</v>
       </c>
-      <c r="N57" s="14">
+      <c r="N57" s="8">
         <v>354807</v>
       </c>
-      <c r="O57" s="14">
+      <c r="O57" s="8">
         <v>356140</v>
       </c>
-      <c r="P57" s="14">
+      <c r="P57" s="8">
         <v>357343</v>
       </c>
-      <c r="Q57" s="14">
+      <c r="Q57" s="8">
         <v>358080</v>
       </c>
-      <c r="R57" s="14">
+      <c r="R57" s="8">
         <v>359471</v>
       </c>
       <c r="S57" s="15">
@@ -4132,56 +4191,56 @@
         <v>0.57834985297840436</v>
       </c>
     </row>
-    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B58" s="13" t="s">
+    <row r="58" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C58" s="14">
+      <c r="C58" s="8">
         <v>132401</v>
       </c>
-      <c r="D58" s="14">
+      <c r="D58" s="8">
         <v>133104</v>
       </c>
-      <c r="E58" s="14">
+      <c r="E58" s="8">
         <v>134404</v>
       </c>
-      <c r="F58" s="14">
+      <c r="F58" s="8">
         <v>134506</v>
       </c>
-      <c r="G58" s="14">
+      <c r="G58" s="8">
         <v>134838</v>
       </c>
-      <c r="H58" s="14">
+      <c r="H58" s="8">
         <v>135374</v>
       </c>
-      <c r="I58" s="14">
+      <c r="I58" s="8">
         <v>132752</v>
       </c>
-      <c r="J58" s="14">
+      <c r="J58" s="8">
         <v>133462</v>
       </c>
-      <c r="K58" s="14">
+      <c r="K58" s="8">
         <v>134188</v>
       </c>
-      <c r="L58" s="14">
+      <c r="L58" s="8">
         <v>136184</v>
       </c>
-      <c r="M58" s="14">
+      <c r="M58" s="8">
         <v>137866</v>
       </c>
-      <c r="N58" s="14">
+      <c r="N58" s="8">
         <v>139671</v>
       </c>
-      <c r="O58" s="14">
+      <c r="O58" s="8">
         <v>140540</v>
       </c>
-      <c r="P58" s="14">
+      <c r="P58" s="8">
         <v>141598</v>
       </c>
-      <c r="Q58" s="14">
+      <c r="Q58" s="8">
         <v>142814</v>
       </c>
-      <c r="R58" s="14">
+      <c r="R58" s="8">
         <v>143698</v>
       </c>
       <c r="S58" s="15">
@@ -4197,56 +4256,56 @@
         <v>0.77036562791409757</v>
       </c>
     </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B59" s="13" t="s">
+    <row r="59" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C59" s="14">
+      <c r="C59" s="8">
         <v>93725</v>
       </c>
-      <c r="D59" s="14">
+      <c r="D59" s="8">
         <v>93094</v>
       </c>
-      <c r="E59" s="14">
+      <c r="E59" s="8">
         <v>92622</v>
       </c>
-      <c r="F59" s="14">
+      <c r="F59" s="8">
         <v>91968</v>
       </c>
-      <c r="G59" s="14">
+      <c r="G59" s="8">
         <v>91228</v>
       </c>
-      <c r="H59" s="14">
+      <c r="H59" s="8">
         <v>90772</v>
       </c>
-      <c r="I59" s="14">
+      <c r="I59" s="8">
         <v>89527</v>
       </c>
-      <c r="J59" s="14">
+      <c r="J59" s="8">
         <v>89126</v>
       </c>
-      <c r="K59" s="14">
+      <c r="K59" s="8">
         <v>88831</v>
       </c>
-      <c r="L59" s="14">
+      <c r="L59" s="8">
         <v>88765</v>
       </c>
-      <c r="M59" s="14">
+      <c r="M59" s="8">
         <v>89239</v>
       </c>
-      <c r="N59" s="14">
+      <c r="N59" s="8">
         <v>89282</v>
       </c>
-      <c r="O59" s="14">
+      <c r="O59" s="8">
         <v>89022</v>
       </c>
-      <c r="P59" s="14">
+      <c r="P59" s="8">
         <v>88624</v>
       </c>
-      <c r="Q59" s="14">
+      <c r="Q59" s="8">
         <v>88583</v>
       </c>
-      <c r="R59" s="14">
+      <c r="R59" s="8">
         <v>88524</v>
       </c>
       <c r="S59" s="15">
@@ -4262,56 +4321,56 @@
         <v>-0.10618589309113913</v>
       </c>
     </row>
-    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B60" s="13" t="s">
+    <row r="60" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="14">
+      <c r="C60" s="8">
         <v>57954</v>
       </c>
-      <c r="D60" s="14">
+      <c r="D60" s="8">
         <v>57829</v>
       </c>
-      <c r="E60" s="14">
+      <c r="E60" s="8">
         <v>57742</v>
       </c>
-      <c r="F60" s="14">
+      <c r="F60" s="8">
         <v>57492</v>
       </c>
-      <c r="G60" s="14">
+      <c r="G60" s="8">
         <v>57391</v>
       </c>
-      <c r="H60" s="14">
+      <c r="H60" s="8">
         <v>57280</v>
       </c>
-      <c r="I60" s="14">
+      <c r="I60" s="8">
         <v>56572</v>
       </c>
-      <c r="J60" s="14">
+      <c r="J60" s="8">
         <v>56362</v>
       </c>
-      <c r="K60" s="14">
+      <c r="K60" s="8">
         <v>56400</v>
       </c>
-      <c r="L60" s="14">
+      <c r="L60" s="8">
         <v>56539</v>
       </c>
-      <c r="M60" s="14">
+      <c r="M60" s="8">
         <v>57173</v>
       </c>
-      <c r="N60" s="14">
+      <c r="N60" s="8">
         <v>56881</v>
       </c>
-      <c r="O60" s="14">
+      <c r="O60" s="8">
         <v>56731</v>
       </c>
-      <c r="P60" s="14">
+      <c r="P60" s="8">
         <v>56882</v>
       </c>
-      <c r="Q60" s="14">
+      <c r="Q60" s="8">
         <v>56926</v>
       </c>
-      <c r="R60" s="14">
+      <c r="R60" s="8">
         <v>57384</v>
       </c>
       <c r="S60" s="15">
@@ -4327,146 +4386,171 @@
         <v>0.12372786839537153</v>
       </c>
     </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B61" s="13" t="s">
+    <row r="61" spans="2:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C61" s="14">
+      <c r="C61" s="20">
         <v>2475459</v>
       </c>
-      <c r="D61" s="14">
+      <c r="D61" s="20">
         <v>2477718</v>
       </c>
-      <c r="E61" s="14">
+      <c r="E61" s="20">
         <v>2480393</v>
       </c>
-      <c r="F61" s="14">
+      <c r="F61" s="20">
         <v>2477771</v>
       </c>
-      <c r="G61" s="14">
+      <c r="G61" s="20">
         <v>2476001</v>
       </c>
-      <c r="H61" s="14">
+      <c r="H61" s="20">
         <v>2477975</v>
       </c>
-      <c r="I61" s="14">
+      <c r="I61" s="20">
         <v>2437727</v>
       </c>
-      <c r="J61" s="14">
+      <c r="J61" s="20">
         <v>2442205</v>
       </c>
-      <c r="K61" s="14">
+      <c r="K61" s="20">
         <v>2446345</v>
       </c>
-      <c r="L61" s="14">
+      <c r="L61" s="20">
         <v>2460857</v>
       </c>
-      <c r="M61" s="14">
+      <c r="M61" s="20">
         <v>2496176</v>
       </c>
-      <c r="N61" s="14">
+      <c r="N61" s="20">
         <v>2506155</v>
       </c>
-      <c r="O61" s="14">
+      <c r="O61" s="20">
         <v>2516457</v>
       </c>
-      <c r="P61" s="14">
+      <c r="P61" s="20">
         <v>2525333</v>
       </c>
-      <c r="Q61" s="14">
+      <c r="Q61" s="20">
         <v>2533993</v>
       </c>
-      <c r="R61" s="14">
+      <c r="R61" s="20">
         <v>2542666</v>
       </c>
-      <c r="S61" s="15">
+      <c r="S61" s="21">
         <v>2554217</v>
       </c>
-      <c r="T61" s="16">
+      <c r="T61" s="22">
         <v>3.1815513809762148</v>
       </c>
-      <c r="U61" s="16">
+      <c r="U61" s="22">
         <v>2.3251966207511008</v>
       </c>
-      <c r="V61" s="16">
+      <c r="V61" s="22">
         <v>0.45428695707576222</v>
       </c>
     </row>
-    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B62" s="13" t="s">
+    <row r="62" spans="2:22" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C62" s="14">
+      <c r="C62" s="20">
         <v>7993946</v>
       </c>
-      <c r="D62" s="14">
+      <c r="D62" s="20">
         <v>7982685</v>
       </c>
-      <c r="E62" s="14">
+      <c r="E62" s="20">
         <v>7971684</v>
       </c>
-      <c r="F62" s="14">
+      <c r="F62" s="20">
         <v>7947244</v>
       </c>
-      <c r="G62" s="14">
+      <c r="G62" s="20">
         <v>7928815</v>
       </c>
-      <c r="H62" s="14">
+      <c r="H62" s="20">
         <v>7918293</v>
       </c>
-      <c r="I62" s="14">
+      <c r="I62" s="20">
         <v>7774253</v>
       </c>
-      <c r="J62" s="14">
+      <c r="J62" s="20">
         <v>7778995</v>
       </c>
-      <c r="K62" s="14">
+      <c r="K62" s="20">
         <v>7790559</v>
       </c>
-      <c r="L62" s="14">
+      <c r="L62" s="20">
         <v>7826739</v>
       </c>
-      <c r="M62" s="14">
+      <c r="M62" s="20">
         <v>7926599</v>
       </c>
-      <c r="N62" s="14">
+      <c r="N62" s="20">
         <v>7945685</v>
       </c>
-      <c r="O62" s="14">
+      <c r="O62" s="20">
         <v>7962775</v>
       </c>
-      <c r="P62" s="14">
+      <c r="P62" s="20">
         <v>7982448</v>
       </c>
-      <c r="Q62" s="14">
+      <c r="Q62" s="20">
         <v>7993608</v>
       </c>
-      <c r="R62" s="14">
+      <c r="R62" s="20">
         <v>8003421</v>
       </c>
-      <c r="S62" s="15">
+      <c r="S62" s="21">
         <v>8027031</v>
       </c>
-      <c r="T62" s="16">
+      <c r="T62" s="22">
         <v>0.41387570043630517</v>
       </c>
-      <c r="U62" s="16">
+      <c r="U62" s="22">
         <v>1.2670251137972288</v>
       </c>
-      <c r="V62" s="16">
+      <c r="V62" s="22">
         <v>0.29499885111629137</v>
       </c>
     </row>
-    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B64" t="str">
+    <row r="63" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="17" t="str">
         <f>[1]A1_2021_Berechnung!B64</f>
         <v>1) Im Berichtsjahr 2011 erfolgte die Umstellung auf die Ergebnisse des Zensus 2011 als neue Basis für die Bevölkerungsfortschreibung. Aufgrund der unterschiedlichen Fortschreibungsbasis ist die Vergleichbarkeit der einzelnen Jahre untereinander eingeschränkt.</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="str">
+    <row r="65" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="18" t="str">
         <f>[1]A1_2021_Berechnung!B67</f>
         <v>Quelle: Bevölkerungsfortschreibung</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="18"/>
+    </row>
+    <row r="68" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4478,7 +4562,7 @@
     <mergeCell ref="T9:V9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B70" r:id="rId1" display="https://www.integrationsmonitoring.niedersachsen.de." xr:uid="{7EC4A8D4-AF5C-4D17-8889-A4A4C1218B78}"/>
+    <hyperlink ref="B71" r:id="rId1" xr:uid="{639D6324-D255-4C1A-82ED-A3BD4312C8D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>